<commit_message>
Edited the pre-req tree
</commit_message>
<xml_diff>
--- a/Data/university_courses/nus_dsa_mods.xlsx
+++ b/Data/university_courses/nus_dsa_mods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melodytan/Library/CloudStorage/OneDrive-NationalUniversityofSingapore/Y3S2/DSA3101/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unu_Stuff\Y3S2\DSA3101\Team_Project\Data\university_courses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5758800-B1EF-ED47-99D2-1E3F8BC0C852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEAA722-DF9C-46C4-B0ED-8A7C538B7164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{32D72EFF-C19C-904F-8F8F-F6B35A9D86F4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{32D72EFF-C19C-904F-8F8F-F6B35A9D86F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="243">
   <si>
     <t>mod_code</t>
   </si>
@@ -104,9 +104,6 @@
     <t>https://nusmods.com/modules/DSA1101/introduction-to-data-science</t>
   </si>
   <si>
-    <t>MA2001</t>
-  </si>
-  <si>
     <t>Linear Algebra I</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>https://nusmods.com/modules/MA2001/linear-algebra-i</t>
   </si>
   <si>
-    <t>MA2002</t>
-  </si>
-  <si>
     <t>Calculus</t>
   </si>
   <si>
@@ -161,9 +155,6 @@
     <t>Data visualisation is an essential tool for data analytics. This module is an introduction to data cleaning, exploration, analysis and visualisation. Students will learn how to take raw data, extract meaningful information, use statistical tools, and make visualisations. Topics include: programming in R, introduction to data storage systems, data manipulation, exploratory data analysis, dimension reduction, statistical graphics for univariate, multivariate (high-dimensional), temporal and spatial data, basic design principles and critical evaluation of visual displays of data.</t>
   </si>
   <si>
-    <t>BT1101/DSA1101/DSE1101/GEA1000/IE1111R/ST1131, GER1000, MA2401/MA1101R/MA1311/MA1508E/MA1513/MA2001, MA2216/ST2334</t>
-  </si>
-  <si>
     <t>https://nusmods.com/modules/DSA2101/essential-data-analytics-tools-data-visualisation</t>
   </si>
   <si>
@@ -176,9 +167,6 @@
     <t>This module aims at introducing basic concepts and wellestablished numerical methods that are very related to the computing foundation of data science and analytics. The emphasis is on the tight integration of numerical algorithms, implementation in industrial programming language, and examination on practical examples drawn from various disciplines related to data science. Major topics include: computer arithmetic, matrix multiplication, numerical methods for solving linear systems, least squares method, interpolation, concrete implementations in industrial program language, and sample applications related to data science.</t>
   </si>
   <si>
-    <t>MA1101R/MA1508E/MA1513/MA2001, MA1102R/MA1312/MA1505/MA1511/MA1521/MA2002</t>
-  </si>
-  <si>
     <t>MA2213</t>
   </si>
   <si>
@@ -194,33 +182,12 @@
     <t>This module applies advanced calculus to practical mathematical problems, and is for students with advanced calculus background and with interest in the applications of calculus. Major topics Sequences, series, power series. Vector algebra in R2 and R3. Scalar- and vector-valued functions of several variables. Partial derivatives, total differentials. Mean value Theorem. Taylor's formula. Jacobian. Chain rule. Lagrange multiplier. Multiple integrals.</t>
   </si>
   <si>
-    <t>MA1102R/MA1312/MA1421/MA1521/MA2002</t>
-  </si>
-  <si>
     <t>MA1104/MA1505/MA1507/MA1511/MA2104/MA2108/MA2108S</t>
   </si>
   <si>
     <t>https://nusmods.com/modules/MA2311/techniques-in-advanced-calculus</t>
   </si>
   <si>
-    <t>MA2104</t>
-  </si>
-  <si>
-    <t>Multivariable Calculus</t>
-  </si>
-  <si>
-    <t>This is a module on the calculus of functions of several real variables, applications of which abound in mathematics, the physical sciences and engineering. The aim is for students to acquire computational skills, ability for 2- and 3-D visualisation and to understand conceptually fundamental results such as Green’s Theorem, Stokes’ Theorem and the Divergence Theorem. Major topics Euclidean distance and elementary topological concepts in Rn, limit and continuity, implicit functions. Partial differentiation, differentiable functions, differentials, chain rules, directional derivatives, gradients, mean value theorem, Taylor’s formula, extreme value theorem, Lagrange multipliers. Multiple integrals and iterated integrals, change of order of integration, applications, Jacobian matrix, change of variables in multiple integrals. Line integrals and Green’s theorem. Surface integrals, Stokes’ Theorem, Divergence Theorem.</t>
-  </si>
-  <si>
-    <t>MA1102R/MA1505/MA1511/MA1521/MA2002</t>
-  </si>
-  <si>
-    <t>MA1104/MA1507/MA2311/YSC2252</t>
-  </si>
-  <si>
-    <t>https://nusmods.com/modules/MA2104/multivariable-calculus</t>
-  </si>
-  <si>
     <t>ST2131</t>
   </si>
   <si>
@@ -233,9 +200,6 @@
     <t>This module gives an elementary introduction to probability theory for students with knowledge of elementary calculus. It will cover not only the mathematics of probability theory but will work through diverse examples to illustrate the wide scope of applicability of probability, such as in engineering and computing, social and management sciences. Topics covered are counting methods, sample space and events, axioms of probability, conditional probability, independence, random variables, discrete and continuous distributions, joint and marginal distributions, conditional distribution, independence of random variables, expectation, conditional expectation, moment generating function, central limit theorem, and weak law of large numbers.</t>
   </si>
   <si>
-    <t>MA1102R/MA1312/MA1505C/MA1507/MA1511</t>
-  </si>
-  <si>
     <t>https://nusmods.com/modules/ST2131/probability</t>
   </si>
   <si>
@@ -248,9 +212,6 @@
     <t>This module introduces students to the theoretical underpinnings of statistical methodology and concentrates on inferential procedures within the framework of parametric models. Topic include: random sample and statistics, method of moments, maximum likelihood estimate, Fisher information, sufficiency and completeness, consistency and unbiasedness, sampling distributions, x2-, t- and Fdistributions, confidence intervals, exact and asymptotic pivotal method, concepts of hypothesis testing, likelihood ratio test, Neyman-Pearson lemma. This module is targeted at students who are interested in Statistic and are able to meet the prerequisite.</t>
   </si>
   <si>
-    <t>ST2334/ST2131</t>
-  </si>
-  <si>
     <t>CE2407/MA2216/ST2334/YSC2243/MA2116</t>
   </si>
   <si>
@@ -266,9 +227,6 @@
     <t>This module introduces basic concepts and algorithms in machine learning and neural networks. The main reason for studying computational learning is to make better use of powerful computers to learn knowledge (or regularities) from the raw data. The ultimate objective is to build self-learning systems to relieve human from some of already-too-many programming tasks. At the end of the course, students are expected to be familiar with the theories and paradigms of computational learning, and capable of implementing basic learning systems.</t>
   </si>
   <si>
-    <t>CS2040/CS2040C/CS2040S/YSC2229,  EE2012/EE2012A/MA2116/MA2216/YSC2243,  MA1511/MA1512/MA1101R, MA1102R/MA1521</t>
-  </si>
-  <si>
     <t>BT4240/CS2109S/CS3264/DMX1401AI</t>
   </si>
   <si>
@@ -299,9 +257,6 @@
     <t>Essential Data Analytics Tools: Convex Optimisation</t>
   </si>
   <si>
-    <t>CS1010, MA1101R/MA1508E/MA1513/MA2001, MA1505/MA1511/MA2104/MA2311</t>
-  </si>
-  <si>
     <t>MA3236</t>
   </si>
   <si>
@@ -317,9 +272,6 @@
     <t>This module focuses on data analysis using multiple regression models. Topics include simple linear regression, multiple regression, model building and regression diagnostics. One and two factor analysis of variance, analysis of covariance, linear model as special case of generalized linear model. This module is targeted at students who are interested in Statistics and are able to meet the pre-requisites.</t>
   </si>
   <si>
-    <t>ST2334/ST2131/MA2116/MA2216</t>
-  </si>
-  <si>
     <t>EC3303/ST2335</t>
   </si>
   <si>
@@ -330,9 +282,6 @@
   </si>
   <si>
     <t>Honours Project in Data Science and Analytics</t>
-  </si>
-  <si>
-    <t>CS1010/CS1010E/CS1010J/CS1010S, DSA1101, MA1101R/MA2001, CS2040, DSA2101, DSA2102, MA2311/MA2104, ST2131/MA2116/MA2216, ST2132, CS3244, DSA3101, DSA3102, ST3131</t>
   </si>
   <si>
     <t>The objectives of the module are to develop skills for independent data-driven research and to promote the application of novel problem-solving strategies in data science. On completion of the module, students should be able to demonstrate an appreciation of the current state of knowledge in a particular field of research, to master the techniques required for the study of a research question, and to communicate research findings clearly and concisely in written and spoken English.</t>
@@ -354,9 +303,6 @@
     <t>Applied Project in Data Science and Analytics</t>
   </si>
   <si>
-    <t>CS1010/CS1010E/CS1010J/CS1010S, DSA1101, MA1101R/MA2001, CS2040, DSA2101, DSA2102, MA2311/MA2104, ST2131/MA2116/MA2216, ST2132, CS3244, DSA3101, DSA3102, ST3131, MA1102R/MA2002</t>
-  </si>
-  <si>
     <t>DSA4199/DSA4299C</t>
   </si>
   <si>
@@ -384,9 +330,6 @@
     <t>Optimisation for Large-Scale Data-Driven Inference</t>
   </si>
   <si>
-    <t>MA1101R/MA2001, MA2104/MA2311, ST2132</t>
-  </si>
-  <si>
     <t>https://nusmods.com/modules/DSA4212/optimisation-for-large-scale-data-driven-inference</t>
   </si>
   <si>
@@ -399,9 +342,6 @@
     <t>The practice of data science involves sense-making, the ability to formulate problems or hypotheses in real-world situations. Only when algorithms and technology are applied to meaningful problems or hypotheses can useful information be extracted from data for making decisions. This module is conducted as a series of hackathons: data scientists from partnering organisations in the health and medicine sector provide the real-world situations and data which will enable students to gain practical experience in (i) formulating problems, (ii) solving them by applying, or developing and implementing, appropriate data-analytic tools and techniques, and (iii) communicating findings and insights gained clearly.</t>
   </si>
   <si>
-    <t>CS3244, DSA1101</t>
-  </si>
-  <si>
     <t>DSA4262A/DSA4262B</t>
   </si>
   <si>
@@ -417,9 +357,6 @@
     <t>The practice of data science involves sense-making, the ability to formulate problems or hypotheses in real-world situations. Only when algorithms and technology are applied to meaningful problems or hypotheses can useful information be extracted from data for making decisions. This module is conducted as a series of hackathons data scientists from partnering organisations in the business and commerce sector provide the real-world situations and data which will enable students to gain practical experience in (i) formulating problems, (ii) solving them by applying, or developing and implementing, appropriate data-analytic tools and techniques, and (iii) communicating findings and insights gained clearly.</t>
   </si>
   <si>
-    <t>CS3244, DSA1102</t>
-  </si>
-  <si>
     <t>DSA4263A/DSA4263B</t>
   </si>
   <si>
@@ -435,9 +372,6 @@
     <t>The practice of data science involves sense-making, the ability to formulate problems or hypotheses in real-world situations. Only when algorithms and technology are applied to meaningful problems or hypotheses can useful information be extracted from data for making decisions. This module is conducted as a series of hackathons: data scientists from partnering organisations in the science and technology sector provide the real-world situations and data which will enable students to gain practical experience in (i) formulating problems, (ii) solving them by applying, or developing and implementing, appropriate data-analytic tools and techniques, and (iii) communicating findings and insights gained clearly.</t>
   </si>
   <si>
-    <t>CS3244, DSA1103</t>
-  </si>
-  <si>
     <t>DSA4266A/DSA4266B</t>
   </si>
   <si>
@@ -450,9 +384,6 @@
     <t>Optimization principles are of undisputed importance in modern design and system operation. The objective of this course is to present these principles and illustrate how algorithms can be designed from the mathematical theories for solving optimization problems. Major topics: Fundamentals, unconstrained optimization: one-dimensional search, Newton-Raphson method, gradient method, constrained optimization: Lagrangian multipliers method, Karush-Kuhn-Tucker optimality conditions, Lagrangian duality and saddle point optimality conditions, convex programming: Frank-Wolfe method.</t>
   </si>
   <si>
-    <t>MA1505/MA1506/MA1507/MA1511/MA2104/MA2311</t>
-  </si>
-  <si>
     <t>DSA3102/DSC3214/DSN3701</t>
   </si>
   <si>
@@ -480,12 +411,6 @@
     <t>This course aims at presenting important mathematical concepts and computational methods that are often used for modelling and analysis of big data sets and complex networks. The emphasis is on mathematical modelling and computational methods for practical problems in data science. Major topics include: basics on convex analysis, numerical methods for large-scale convex problems, dimensionality reduction, numerical methods for machine learning, kernel methods for pattern analysis, sparse coding and dictionary learning.</t>
   </si>
   <si>
-    <t>MA1101/MA1101R/MA1306/MA1506/MA1508/MA1311/MA1508E/MA1513/MA2001</t>
-  </si>
-  <si>
-    <t>DSA2102/MA2213, MA2216/ST2131/ST2334</t>
-  </si>
-  <si>
     <t>CS5339/DSA5102</t>
   </si>
   <si>
@@ -504,9 +429,6 @@
     <t>This module covers common designs of experiments and their analysis. Topics include basic experimental designs, analysis of one-way and two way layout data, multiple comparisons, factorial designs, 2k-factorial designs, blocking and confounding, fractional factorial design and nested designs. This module is targeted at students who are interested in Statistics and are able to meet the pre-requisites.</t>
   </si>
   <si>
-    <t>ST2132/ST2334</t>
-  </si>
-  <si>
     <t>https://nusmods.com/modules/ST3232/design-analysis-of-experiments</t>
   </si>
   <si>
@@ -534,9 +456,6 @@
     <t>This module gives an introduction to the design of sample surveys and estimation procedures, with emphasis on practical applications in survey sampling. Topics include planning of surveys, questionnaire construction, methods of data collection, fieldwork procedures, sources of errors, basic ideas of sampling, simple random sampling, stratified, systematic, replicated, cluster and quota sampling, sample size determination and cost. This module is targeted at students who are interested in Statistics and are able to meet the pre-requisites.</t>
   </si>
   <si>
-    <t>ST2334/ST2131/MA2116</t>
-  </si>
-  <si>
     <t>ST4250</t>
   </si>
   <si>
@@ -564,9 +483,6 @@
     <t>The advent of fast and inexpensive computational power has facilitated the description of real phenomenon using realistic stochastic models which can be analysed using simulation studies. This module teaches students how to analyse a model by use of a simulation study and the topics include pseudorandom number generation, generating discrete and continuous random variables, simulating discrete events, statistical analysis of simulated data, variance reduction, Markov Chain Monte Carlo methods. It also covers topics in stochastic optimisation such as simulated annealing. This module is targeted at students who are interested in Statistics and are able to meet the prerequisites.</t>
   </si>
   <si>
-    <t xml:space="preserve">ST2334/MA2216/MA2116/ST2131, CS1010/CS1010E/CS1010S </t>
-  </si>
-  <si>
     <t>https://nusmods.com/modules/ST3247/simulation</t>
   </si>
   <si>
@@ -579,9 +495,6 @@
     <t>Statistical learning is a large collection of computer-based modelling and prediction tools with applications in diverse fields including business, medicine, astrophysics, and public policy. This series of two modules covers many of the popular approaches for a variety of statistical problems. There is heavy emphasis on the implementation of these methods on real-world data sets in the popular statistical software package R. Part I gives a broad overview of the common problems as well as their most popular approaches. Topics include linear regression model and its extensions, classification methods, resampling methods, regularisation and model selection, principal components and clustering methods.</t>
   </si>
   <si>
-    <t xml:space="preserve"> ST2132/ST2334</t>
-  </si>
-  <si>
     <t>ST4240/YSC4216</t>
   </si>
   <si>
@@ -621,9 +534,6 @@
     <t>Statistical Learning is a large collection of computer-based modelling and prediction tools with applications in diverse fields including business, medicine, astrophysics, and public policy. This series of two modules covers many of the popular approaches for a variety of statistical problems. There is heavy emphasis on the implementation of these methods on real-world data sets in the popular statistical software package R. Part II builds on the knowledge in Part I, introducing more tools as well as generalising and extending some of the tools covered in Part I using entirely different approaches. Topics include non-parametric smoothing methods, tree-based methods, support vector machines, neural networks and ensemble learning.</t>
   </si>
   <si>
-    <t xml:space="preserve"> ST3131/ST3248</t>
-  </si>
-  <si>
     <t>https://nusmods.com/modules/ST4248/statistical-learning-ii</t>
   </si>
   <si>
@@ -636,9 +546,6 @@
     <t>The aim of this module is to provide an introduction to the field of parallel computing with hands-on parallel programming experience on real parallel machines. The module is divided into four parts parallel computation models and parallelism, parallel architectures, parallel algorithm design and programming, and new parallel computing models. Topics includes theory of parallelism and models; shared-memory architectures; distributed-memory architectures; data parallel architectures; interconnection networks, topologies and basic of communication operations; principles of parallel algorithm design; performance and scalability of parallel programs, overview of new parallel computing models such as grid, cloud, GPGPU.</t>
   </si>
   <si>
-    <t>CG2007/CG2028/CS2100/EE2024/EE2028</t>
-  </si>
-  <si>
     <t>https://nusmods.com/modules/CS3210/parallel-computing</t>
   </si>
   <si>
@@ -651,12 +558,6 @@
     <t>This system-oriented module provides an in-depth study of the concepts and implementation issues related to database management systems. It first covers the physical implementation of the relational data model, which includes storage management, access methods, query processing, and optimisation. Then it covers issues and techniques dealing with multi-user application environments, namely, transactions, concurrency control, and recovery. The third part covers advanced topics such as on-line analytical processing, in-memory databases, and column stores.</t>
   </si>
   <si>
-    <t xml:space="preserve">CS2010/CS2020/CS2040/CS2040C/CS2040S </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CS2102/IT2002</t>
-  </si>
-  <si>
     <t>https://nusmods.com/modules/CS3223/database-systems-implementation</t>
   </si>
   <si>
@@ -669,9 +570,6 @@
     <t>This module introduces different techniques of designing and analysing algorithms. Students will learn about the framework for algorithm analysis, for example, lower bound arguments, average case analysis, and the theory of NP-completeness. In addition, students are exposed to various algorithm design paradigms. The module serves two purposes: to improve the students' ability to design algorithms in different areas, and to prepare students for the study of more advanced algorithms. The module covers lower and upper bounds, recurrences, basic algorithm paradigms (such as prune-and-search, dynamic programming, branch-and-bound, graph traversal, and randomised approaches), amortized analysis, NP-completeness, and some selected advanced topics.</t>
   </si>
   <si>
-    <t xml:space="preserve">CS2010/CS2020/CS2040/CS2040C/CS2040S/YSC2229 </t>
-  </si>
-  <si>
     <t>https://nusmods.com/modules/CS3230/design-and-analysis-of-algorithms</t>
   </si>
   <si>
@@ -684,9 +582,6 @@
     <t>The module introduces the basic concepts in search and knowledge representation as well as to a number of sub-areas of artificial intelligence. It focuses on covering the essential concepts in AI. The module covers Turing test, blind search, iterative deepening, production systems, heuristic search, A* algorithm, minimax and alpha-beta procedures, predicate and first-order logic, resolution refutation, non-monotonic reasoning, assumption-based truth maintenance systems, inheritance hierarchies, the frame problem, certainly factors, Bayes' rule, frames and semantic nets, planning, learning, natural language, vision, and expert systems and LISP.</t>
   </si>
   <si>
-    <t xml:space="preserve"> CS2040/CS2040C/CS2040S/YSC2229, CS1231/CS1231S/MA1100/MA1100T</t>
-  </si>
-  <si>
     <t xml:space="preserve"> CS2109S/CS3263</t>
   </si>
   <si>
@@ -732,9 +627,6 @@
     <t>This course will examine some fundamental issues in parallel programming and distributed computing, and the relationships between the two. Parallel programming: mutual exclusion, semaphores, consistency, wait-free synchronization. Distributed computing: time, global state, snapshots, message ordering. Relationships: consensus, fault-tolerance, transactions, self-stabilization.</t>
   </si>
   <si>
-    <t xml:space="preserve"> CS3210/CS3230</t>
-  </si>
-  <si>
     <t>https://nusmods.com/modules/CS4231/parallel-and-distributed-algorithms</t>
   </si>
   <si>
@@ -747,9 +639,6 @@
     <t>This module covers common algorithmic techniques for solving optimisation problems, and introduces students to approaches for finding good-enough solutions to NP-hard problems. Topics covered include linear and integer programming, network flow algorithms, local search heuristics, approximation algorithms, and randomized algorithms. Through analysis and application of the techniques to a variety of canonical problems, students develop confidence to (i) appropriately model a given optimisation problem, (ii) apply appropriate algorithmic techniques to solve the problem, (iii) analyse the properties of the problem and candidate algorithms, such as time and space complexity, convergence, approximability, and optimality bound.</t>
   </si>
   <si>
-    <t>MA1101R/MA1311/MA1508E/MA2001/YSC2232, CS3230/YSC3203</t>
-  </si>
-  <si>
     <t>https://nusmods.com/modules/CS4234/optimisation-algorithms</t>
   </si>
   <si>
@@ -762,9 +651,6 @@
     <t>This module is for undergraduates who are interested in computer vision and its applications. It covers (a) the basic skills needed in handling images and videos, (b) the basic theories needed to understand geometrical computer vision, and (c) pattern recognition. Topics covered in image handling include contrast stretch, histogram equalization, noise removal, and color space. Topics covered in geometrical vision include affine transform, vanishing points, camera projection models, homography, camera calibration, rotation representations including quaternions, epipolar geometry, binocular stereo, structure from motion. Topics covered for pattern recognition include principal component analysis.</t>
   </si>
   <si>
-    <t>MA1101R/MA1311/MA1508E/MA1513/MA2001/YSC2232, MA2216"/"ST1131A"/EE2012/EE2012A/MA2116/ST1131/ST1232/ST2131/ST2334/YSC2243, CS1020/CS1020E/CS2020/CS2030/CS2030S/CS2113/CS2113T/ CS2040/CS2040C/CS2040S/YSC2229, MA1102R/MA1507/MA1505/MA1521/MA2002/YSC1216/MA1511/MA1512</t>
-  </si>
-  <si>
     <t>EE4212/EE4704</t>
   </si>
   <si>
@@ -780,9 +666,6 @@
     <t>Natural Language Processing</t>
   </si>
   <si>
-    <t>CS2109S/CS3243, MA2216/EE2012/EE2012A/MA2116/ST2131/ST2334/YSC2243, MA1102R/MA1507/MA1505/MA1521/MA2002/YSC1216/MA1511/MA1512</t>
-  </si>
-  <si>
     <t>https://nusmods.com/modules/CS4248/natural-language-processing</t>
   </si>
   <si>
@@ -795,18 +678,12 @@
     <t>The module covers modelling methods that are suitable for reasoning with uncertainty. The main focus will be on probabilistic models including Bayesian networks and Markov networks. Topics include representing conditional independence, building graphical models, inference using graphical models and learning from data. Selected applications in various domains such as speech, vision, natural language processing, medical informatics, bioinformatics, data mining and others will be discussed.</t>
   </si>
   <si>
-    <t>CS3243/CS3263, EE2012/EE2012A/ST2132/ST2334/MA2116/MA2216/ST2131, DSC2008/ST1131/ST1131A/ST1232</t>
-  </si>
-  <si>
     <t>https://nusmods.com/modules/CS5340/uncertainty-modelling-in-ai</t>
   </si>
   <si>
     <t>MA4230</t>
   </si>
   <si>
-    <t>MA2101/MA2101S, DSA2102/MA2213</t>
-  </si>
-  <si>
     <t>https://nusmods.com/modules/MA4230/matrix-computation</t>
   </si>
   <si>
@@ -814,6 +691,81 @@
   </si>
   <si>
     <t>Matrix Computation</t>
+  </si>
+  <si>
+    <t>DSA1101, GER1000, MA1101R,ST2131/ MA2216</t>
+  </si>
+  <si>
+    <t>MA1101R</t>
+  </si>
+  <si>
+    <t>MA11012R</t>
+  </si>
+  <si>
+    <t>MA1101R, MA1102R</t>
+  </si>
+  <si>
+    <t>MA1102R</t>
+  </si>
+  <si>
+    <t>CS2040, ST2131 MA1101R, MA1102R</t>
+  </si>
+  <si>
+    <t>CS1010, MA1101R, MA2311</t>
+  </si>
+  <si>
+    <t>CS1010, DSA1101, MA1101R CS2040, DSA2101, DSA2102, MA2311, ST2131, ST2132, CS3244, DSA3101, DSA3102, ST3131</t>
+  </si>
+  <si>
+    <t>MA1101R, MA2311, ST2132</t>
+  </si>
+  <si>
+    <t>CS3244, DSA3101</t>
+  </si>
+  <si>
+    <t>DSA2102,ST2131</t>
+  </si>
+  <si>
+    <t>ST2132/</t>
+  </si>
+  <si>
+    <t>ST2131, CS1010</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ST2132</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ST3131, ST3248</t>
+  </si>
+  <si>
+    <t>CS2100</t>
+  </si>
+  <si>
+    <t>CS2040, CS2102</t>
+  </si>
+  <si>
+    <t>CS2040, CS1231</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CS2102</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CS3210, CS3230</t>
+  </si>
+  <si>
+    <t>MA1101R,  CS3230</t>
+  </si>
+  <si>
+    <t>MA1101R, ST2131, CS2030, MA1102R, CS2040</t>
+  </si>
+  <si>
+    <t>CS3243, ST2131, MA1102R</t>
+  </si>
+  <si>
+    <t>CS3243, ST2132,ST2131</t>
+  </si>
+  <si>
+    <t>MA2101, DSA2102</t>
   </si>
 </sst>
 </file>
@@ -1187,23 +1139,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC54D492-7187-A743-B199-19558CEA035D}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M47" sqref="M47"/>
+      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="21.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
     <col min="5" max="5" width="44.1640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="7" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="9.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1235,7 +1189,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="340" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="217" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1264,7 +1218,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="248" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1296,21 +1250,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="340" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="248" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>219</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -1322,27 +1276,27 @@
         <v>19</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="372" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:10" ht="232.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>220</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -1354,27 +1308,27 @@
         <v>19</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="119" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
@@ -1386,27 +1340,27 @@
         <v>9</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="186" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="238" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -1415,59 +1369,59 @@
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="217" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="238" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="155" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="221" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -1476,30 +1430,30 @@
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>52</v>
+        <v>222</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="340" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="248" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -1508,216 +1462,216 @@
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="J10" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="372" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="217" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="201.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="J12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1" t="s">
+    </row>
+    <row r="13" spans="1:10" ht="124" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="238" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="272" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="B13" s="1">
         <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
       <c r="G13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="187" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="155" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B14" s="1">
         <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
       </c>
       <c r="G14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>81</v>
+        <v>224</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="170" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="124" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B15" s="1">
         <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="201.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="1">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="201.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="153" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="1">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="323" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="B17" s="1">
         <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
@@ -1726,62 +1680,59 @@
         <v>0</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>98</v>
+        <v>225</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="356" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="263.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="B18" s="1">
         <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
       </c>
       <c r="G18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="388" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="186" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B19" s="1">
         <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
@@ -1790,56 +1741,59 @@
         <v>1</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>90</v>
+        <v>226</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="255" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="232.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B20" s="1">
         <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
       </c>
       <c r="G20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>115</v>
+        <v>227</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="356" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="232.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B21" s="1">
         <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
@@ -1848,30 +1802,30 @@
         <v>0</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>120</v>
+        <v>227</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="356" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="232.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B22" s="1">
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
@@ -1880,62 +1834,62 @@
         <v>0</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>126</v>
+        <v>227</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="201.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="B23" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="F23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>132</v>
+        <v>45</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="221" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="B24" s="1">
         <v>3</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -1944,216 +1898,213 @@
         <v>1</v>
       </c>
       <c r="H24" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="186" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" s="1">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="1">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="170.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" s="1">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="D28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="155" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="B29" s="1">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B25" s="1">
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="232.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="1">
         <v>3</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F25" s="1">
-        <v>0</v>
-      </c>
-      <c r="G25" s="1">
-        <v>1</v>
-      </c>
-      <c r="H25" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="204" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B26" s="1">
-        <v>4</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F26" s="1">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1">
-        <v>1</v>
-      </c>
-      <c r="H26" s="1" t="s">
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J30" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="I26" s="1" t="s">
+    </row>
+    <row r="31" spans="1:10" ht="232.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="153" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B27" s="1">
-        <v>3</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F27" s="1">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1">
-        <v>1</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="119" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B28" s="1">
-        <v>4</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F28" s="1">
-        <v>1</v>
-      </c>
-      <c r="G28" s="1">
-        <v>1</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="204" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B29" s="1">
-        <v>3</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="F29" s="1">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1">
-        <v>1</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="187" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B30" s="1">
-        <v>4</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F30" s="1">
-        <v>1</v>
-      </c>
-      <c r="G30" s="1">
-        <v>1</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="255" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="B31" s="1">
         <v>3</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
@@ -2162,27 +2113,30 @@
         <v>1</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>175</v>
+        <v>231</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="248" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="B32" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="F32" s="1">
         <v>1</v>
@@ -2191,30 +2145,27 @@
         <v>1</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>181</v>
+        <v>55</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="289" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="155" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="B33" s="1">
         <v>4</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
@@ -2223,27 +2174,27 @@
         <v>1</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="187" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="248" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="B34" s="1">
         <v>4</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
@@ -2252,27 +2203,30 @@
         <v>1</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>67</v>
+        <v>232</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="232.5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="B35" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="F35" s="1">
         <v>1</v>
@@ -2281,30 +2235,27 @@
         <v>1</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>181</v>
+        <v>233</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="255" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="201.5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="B36" s="1">
         <v>3</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="F36" s="1">
         <v>1</v>
@@ -2313,27 +2264,27 @@
         <v>1</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>199</v>
+        <v>234</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="221" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="248" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>201</v>
+        <v>174</v>
       </c>
       <c r="B37" s="1">
         <v>3</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>202</v>
+        <v>175</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
       <c r="F37" s="1">
         <v>1</v>
@@ -2342,30 +2293,27 @@
         <v>1</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>205</v>
+        <v>235</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="217" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="B38" s="1">
         <v>3</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>208</v>
+        <v>179</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="F38" s="1">
         <v>1</v>
@@ -2374,27 +2322,30 @@
         <v>1</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>210</v>
+        <v>235</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="238" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="155" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
       <c r="B39" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>213</v>
+        <v>184</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="F39" s="1">
         <v>1</v>
@@ -2403,30 +2354,30 @@
         <v>1</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>215</v>
+        <v>170</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="187" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="201.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="B40" s="1">
         <v>4</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="F40" s="1">
         <v>1</v>
@@ -2435,30 +2386,30 @@
         <v>1</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>201</v>
+        <v>236</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="238" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="124" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>223</v>
+        <v>193</v>
       </c>
       <c r="B41" s="1">
         <v>4</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>224</v>
+        <v>194</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="F41" s="1">
         <v>1</v>
@@ -2467,30 +2418,27 @@
         <v>1</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="153" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="248" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>228</v>
+        <v>197</v>
       </c>
       <c r="B42" s="1">
         <v>4</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
       <c r="F42" s="1">
         <v>1</v>
@@ -2499,27 +2447,27 @@
         <v>1</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="232.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="B43" s="1">
         <v>4</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
       <c r="F43" s="1">
         <v>1</v>
@@ -2528,59 +2476,59 @@
         <v>1</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>238</v>
+        <v>206</v>
       </c>
       <c r="B44" s="1">
         <v>4</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>239</v>
+        <v>208</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F44" s="1">
-        <v>1</v>
-      </c>
-      <c r="G44" s="1">
-        <v>1</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>242</v>
-      </c>
       <c r="J44" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="255" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
       <c r="B45" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>245</v>
+        <v>212</v>
       </c>
       <c r="F45" s="1">
         <v>1</v>
@@ -2589,27 +2537,27 @@
         <v>1</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="204" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="248" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="B46" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>250</v>
+        <v>217</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>251</v>
+        <v>216</v>
       </c>
       <c r="F46" s="1">
         <v>1</v>
@@ -2618,39 +2566,10 @@
         <v>1</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="272" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="B47" s="1">
-        <v>4</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="F47" s="1">
-        <v>1</v>
-      </c>
-      <c r="G47" s="1">
-        <v>1</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>256</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2664,43 +2583,42 @@
     <hyperlink ref="J7" r:id="rId6" xr:uid="{61403323-BE26-8343-92CD-11863ABA2CA9}"/>
     <hyperlink ref="J8" r:id="rId7" xr:uid="{6E762283-EC21-7B40-BDD0-5C3A4A162FB3}"/>
     <hyperlink ref="J9" r:id="rId8" xr:uid="{8DEF8A07-4A95-0743-91E0-ED38D374021C}"/>
-    <hyperlink ref="J10" r:id="rId9" xr:uid="{7D0416E9-C21C-3D4E-A96B-D080F8DA809B}"/>
-    <hyperlink ref="J11" r:id="rId10" xr:uid="{3970091D-24AC-D949-8C53-4A46DAE197CC}"/>
-    <hyperlink ref="J12" r:id="rId11" xr:uid="{0F4E42DA-E0EF-B849-A90E-809D677EF68E}"/>
-    <hyperlink ref="J13" r:id="rId12" xr:uid="{C3200318-9490-D545-9B1E-9B54AC387B09}"/>
-    <hyperlink ref="J14" r:id="rId13" xr:uid="{4F90DC68-8DE7-7A4C-A32C-9E764BB17A38}"/>
-    <hyperlink ref="J15" r:id="rId14" xr:uid="{8F2F294B-4DDB-1044-BA54-A0505B012444}"/>
-    <hyperlink ref="J16" r:id="rId15" xr:uid="{5AC9EDAF-8DCE-7F44-9DAE-8F4704358928}"/>
-    <hyperlink ref="J17" r:id="rId16" xr:uid="{1A576F3D-ABE9-5E4B-8E8A-0E8415707F54}"/>
-    <hyperlink ref="J18" r:id="rId17" xr:uid="{91DD8113-2BCF-6D49-910E-6CD8A054054D}"/>
-    <hyperlink ref="J19" r:id="rId18" xr:uid="{7B4CE37C-58AA-8247-9B62-1B9C6BDE2611}"/>
-    <hyperlink ref="J20" r:id="rId19" xr:uid="{5F394AFB-B26E-3944-AD42-B9CFA24F50BA}"/>
-    <hyperlink ref="J21" r:id="rId20" xr:uid="{AE931061-0A21-A94E-9A0C-0C9091567F9C}"/>
-    <hyperlink ref="J23" r:id="rId21" xr:uid="{DB4B3E38-CC15-2141-BC2D-99B1958B1C87}"/>
-    <hyperlink ref="J24" r:id="rId22" xr:uid="{55117DDD-1B4C-7E4B-851F-143144A03343}"/>
-    <hyperlink ref="J25" r:id="rId23" xr:uid="{CBB85CA2-C41D-F44D-97B8-1DF24EEC1B5D}"/>
-    <hyperlink ref="J26" r:id="rId24" xr:uid="{484F185B-9B01-1743-941E-91FE220B775D}"/>
-    <hyperlink ref="J27" r:id="rId25" xr:uid="{08C44DD2-8B6E-0D43-B04D-6D8FA4F08FB1}"/>
-    <hyperlink ref="J28" r:id="rId26" xr:uid="{325C7CCF-0AD9-E440-9342-354B2FA85734}"/>
-    <hyperlink ref="J30" r:id="rId27" xr:uid="{645042D2-2C01-1940-8964-165604D9C299}"/>
-    <hyperlink ref="J29" r:id="rId28" xr:uid="{C188A6FA-C789-8745-965B-E9D799547003}"/>
-    <hyperlink ref="J31" r:id="rId29" xr:uid="{06E5EB6A-8E7D-B64E-BDA2-F0DB03F45276}"/>
-    <hyperlink ref="J32" r:id="rId30" xr:uid="{E975B232-9F02-E543-ADA2-3C127EE31E87}"/>
-    <hyperlink ref="J33" r:id="rId31" xr:uid="{326128BB-421A-504C-A068-2F8B8A90D30D}"/>
-    <hyperlink ref="J34" r:id="rId32" xr:uid="{ADE053E8-E2EE-1445-B263-515448F644D9}"/>
-    <hyperlink ref="J35" r:id="rId33" xr:uid="{56ACB0D0-7E13-1443-9AD6-D158B9B142EB}"/>
-    <hyperlink ref="J36" r:id="rId34" xr:uid="{DB738535-76F8-D249-9ABA-5D338CF718CD}"/>
-    <hyperlink ref="J37" r:id="rId35" xr:uid="{CB989806-E7E8-F645-946F-6EDBD2BFC0B8}"/>
-    <hyperlink ref="J38" r:id="rId36" xr:uid="{0EF144F2-06FC-9347-8924-DF3B8A3AAF98}"/>
-    <hyperlink ref="J39" r:id="rId37" xr:uid="{FF2F0D69-380F-6341-9FAC-DFBE4556314F}"/>
-    <hyperlink ref="J40" r:id="rId38" xr:uid="{A50BED31-E1BA-8740-97F3-AF8A76B75F96}"/>
-    <hyperlink ref="J41" r:id="rId39" xr:uid="{5DE6BECA-25A0-6E40-AA95-2B59249E8141}"/>
-    <hyperlink ref="J42" r:id="rId40" xr:uid="{92527368-A9AA-B94D-8C00-034BBB2608B4}"/>
-    <hyperlink ref="J43" r:id="rId41" xr:uid="{9D95F6FF-4FCA-E64C-8C58-BA30F1C4DFE5}"/>
-    <hyperlink ref="J44" r:id="rId42" xr:uid="{1707545F-52FE-A442-9795-BA002AEDE6EE}"/>
-    <hyperlink ref="J45" r:id="rId43" xr:uid="{6A858CE8-90D1-D24A-B5FC-34C028900F81}"/>
-    <hyperlink ref="J46" r:id="rId44" xr:uid="{5AC620F7-EE12-C240-BE62-AB355553C260}"/>
-    <hyperlink ref="J47" r:id="rId45" xr:uid="{4CE5A0C3-57D6-0D46-96C9-F143B25C5A80}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{3970091D-24AC-D949-8C53-4A46DAE197CC}"/>
+    <hyperlink ref="J11" r:id="rId10" xr:uid="{0F4E42DA-E0EF-B849-A90E-809D677EF68E}"/>
+    <hyperlink ref="J12" r:id="rId11" xr:uid="{C3200318-9490-D545-9B1E-9B54AC387B09}"/>
+    <hyperlink ref="J13" r:id="rId12" xr:uid="{4F90DC68-8DE7-7A4C-A32C-9E764BB17A38}"/>
+    <hyperlink ref="J14" r:id="rId13" xr:uid="{8F2F294B-4DDB-1044-BA54-A0505B012444}"/>
+    <hyperlink ref="J15" r:id="rId14" xr:uid="{5AC9EDAF-8DCE-7F44-9DAE-8F4704358928}"/>
+    <hyperlink ref="J16" r:id="rId15" xr:uid="{1A576F3D-ABE9-5E4B-8E8A-0E8415707F54}"/>
+    <hyperlink ref="J17" r:id="rId16" xr:uid="{91DD8113-2BCF-6D49-910E-6CD8A054054D}"/>
+    <hyperlink ref="J18" r:id="rId17" xr:uid="{7B4CE37C-58AA-8247-9B62-1B9C6BDE2611}"/>
+    <hyperlink ref="J19" r:id="rId18" xr:uid="{5F394AFB-B26E-3944-AD42-B9CFA24F50BA}"/>
+    <hyperlink ref="J20" r:id="rId19" xr:uid="{AE931061-0A21-A94E-9A0C-0C9091567F9C}"/>
+    <hyperlink ref="J22" r:id="rId20" xr:uid="{DB4B3E38-CC15-2141-BC2D-99B1958B1C87}"/>
+    <hyperlink ref="J23" r:id="rId21" xr:uid="{55117DDD-1B4C-7E4B-851F-143144A03343}"/>
+    <hyperlink ref="J24" r:id="rId22" xr:uid="{CBB85CA2-C41D-F44D-97B8-1DF24EEC1B5D}"/>
+    <hyperlink ref="J25" r:id="rId23" xr:uid="{484F185B-9B01-1743-941E-91FE220B775D}"/>
+    <hyperlink ref="J26" r:id="rId24" xr:uid="{08C44DD2-8B6E-0D43-B04D-6D8FA4F08FB1}"/>
+    <hyperlink ref="J27" r:id="rId25" xr:uid="{325C7CCF-0AD9-E440-9342-354B2FA85734}"/>
+    <hyperlink ref="J29" r:id="rId26" xr:uid="{645042D2-2C01-1940-8964-165604D9C299}"/>
+    <hyperlink ref="J28" r:id="rId27" xr:uid="{C188A6FA-C789-8745-965B-E9D799547003}"/>
+    <hyperlink ref="J30" r:id="rId28" xr:uid="{06E5EB6A-8E7D-B64E-BDA2-F0DB03F45276}"/>
+    <hyperlink ref="J31" r:id="rId29" xr:uid="{E975B232-9F02-E543-ADA2-3C127EE31E87}"/>
+    <hyperlink ref="J32" r:id="rId30" xr:uid="{326128BB-421A-504C-A068-2F8B8A90D30D}"/>
+    <hyperlink ref="J33" r:id="rId31" xr:uid="{ADE053E8-E2EE-1445-B263-515448F644D9}"/>
+    <hyperlink ref="J34" r:id="rId32" xr:uid="{56ACB0D0-7E13-1443-9AD6-D158B9B142EB}"/>
+    <hyperlink ref="J35" r:id="rId33" xr:uid="{DB738535-76F8-D249-9ABA-5D338CF718CD}"/>
+    <hyperlink ref="J36" r:id="rId34" xr:uid="{CB989806-E7E8-F645-946F-6EDBD2BFC0B8}"/>
+    <hyperlink ref="J37" r:id="rId35" xr:uid="{0EF144F2-06FC-9347-8924-DF3B8A3AAF98}"/>
+    <hyperlink ref="J38" r:id="rId36" xr:uid="{FF2F0D69-380F-6341-9FAC-DFBE4556314F}"/>
+    <hyperlink ref="J39" r:id="rId37" xr:uid="{A50BED31-E1BA-8740-97F3-AF8A76B75F96}"/>
+    <hyperlink ref="J40" r:id="rId38" xr:uid="{5DE6BECA-25A0-6E40-AA95-2B59249E8141}"/>
+    <hyperlink ref="J41" r:id="rId39" xr:uid="{92527368-A9AA-B94D-8C00-034BBB2608B4}"/>
+    <hyperlink ref="J42" r:id="rId40" xr:uid="{9D95F6FF-4FCA-E64C-8C58-BA30F1C4DFE5}"/>
+    <hyperlink ref="J43" r:id="rId41" xr:uid="{1707545F-52FE-A442-9795-BA002AEDE6EE}"/>
+    <hyperlink ref="J44" r:id="rId42" xr:uid="{6A858CE8-90D1-D24A-B5FC-34C028900F81}"/>
+    <hyperlink ref="J45" r:id="rId43" xr:uid="{5AC620F7-EE12-C240-BE62-AB355553C260}"/>
+    <hyperlink ref="J46" r:id="rId44" xr:uid="{4CE5A0C3-57D6-0D46-96C9-F143B25C5A80}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added categories for nus_mods
</commit_message>
<xml_diff>
--- a/Data/university_courses/nus_dsa_mods.xlsx
+++ b/Data/university_courses/nus_dsa_mods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melodytan/Library/CloudStorage/OneDrive-NationalUniversityofSingapore/Y3S2/DSA3101/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melodytan/dsa3101-2220-12-ds/Data/university_courses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5758800-B1EF-ED47-99D2-1E3F8BC0C852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4003E5-33D5-2A4A-B36A-35761BDD616F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{32D72EFF-C19C-904F-8F8F-F6B35A9D86F4}"/>
+    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="16020" xr2:uid="{32D72EFF-C19C-904F-8F8F-F6B35A9D86F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="264">
   <si>
     <t>mod_code</t>
   </si>
@@ -814,6 +814,21 @@
   </si>
   <si>
     <t>Matrix Computation</t>
+  </si>
+  <si>
+    <t>mod_category</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>Data Science and Analytics</t>
+  </si>
+  <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>Statistics</t>
   </si>
 </sst>
 </file>
@@ -1187,11 +1202,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC54D492-7187-A743-B199-19558CEA035D}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M47" sqref="M47"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1203,7 +1218,7 @@
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1234,8 +1249,11 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="340" x14ac:dyDescent="0.2">
+      <c r="K1" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1263,8 +1281,11 @@
       <c r="J2" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+      <c r="K2" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1295,8 +1316,11 @@
       <c r="J3" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="340" x14ac:dyDescent="0.2">
+      <c r="K3" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1327,8 +1351,11 @@
       <c r="J4" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="372" x14ac:dyDescent="0.2">
+      <c r="K4" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -1359,8 +1386,11 @@
       <c r="J5" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="119" x14ac:dyDescent="0.2">
+      <c r="K5" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1391,8 +1421,11 @@
       <c r="J6" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="238" x14ac:dyDescent="0.2">
+      <c r="K6" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
@@ -1420,8 +1453,11 @@
       <c r="J7" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="238" x14ac:dyDescent="0.2">
+      <c r="K7" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -1452,8 +1488,11 @@
       <c r="J8" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="221" x14ac:dyDescent="0.2">
+      <c r="K8" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="170" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>49</v>
       </c>
@@ -1484,8 +1523,11 @@
       <c r="J9" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="340" x14ac:dyDescent="0.2">
+      <c r="K9" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="340" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -1516,8 +1558,11 @@
       <c r="J10" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="372" x14ac:dyDescent="0.2">
+      <c r="K10" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>61</v>
       </c>
@@ -1548,8 +1593,11 @@
       <c r="J11" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="238" x14ac:dyDescent="0.2">
+      <c r="K11" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
@@ -1577,8 +1625,11 @@
       <c r="J12" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+      <c r="K12" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>73</v>
       </c>
@@ -1609,8 +1660,11 @@
       <c r="J13" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="187" x14ac:dyDescent="0.2">
+      <c r="K13" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="136" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>79</v>
       </c>
@@ -1638,8 +1692,11 @@
       <c r="J14" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="170" x14ac:dyDescent="0.2">
+      <c r="K14" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="170" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>85</v>
       </c>
@@ -1670,8 +1727,11 @@
       <c r="J15" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="153" x14ac:dyDescent="0.2">
+      <c r="K15" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="153" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>90</v>
       </c>
@@ -1702,8 +1762,11 @@
       <c r="J16" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="323" x14ac:dyDescent="0.2">
+      <c r="K16" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="323" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>96</v>
       </c>
@@ -1734,8 +1797,11 @@
       <c r="J17" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="356" x14ac:dyDescent="0.2">
+      <c r="K17" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="356" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>103</v>
       </c>
@@ -1766,8 +1832,11 @@
       <c r="J18" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="388" x14ac:dyDescent="0.2">
+      <c r="K18" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>108</v>
       </c>
@@ -1795,8 +1864,11 @@
       <c r="J19" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="255" x14ac:dyDescent="0.2">
+      <c r="K19" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="204" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>112</v>
       </c>
@@ -1824,8 +1896,11 @@
       <c r="J20" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="356" x14ac:dyDescent="0.2">
+      <c r="K20" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>117</v>
       </c>
@@ -1856,8 +1931,11 @@
       <c r="J21" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="356" x14ac:dyDescent="0.2">
+      <c r="K21" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>123</v>
       </c>
@@ -1888,8 +1966,11 @@
       <c r="J22" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+      <c r="K22" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>130</v>
       </c>
@@ -1920,8 +2001,11 @@
       <c r="J23" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="221" x14ac:dyDescent="0.2">
+      <c r="K23" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="221" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>88</v>
       </c>
@@ -1952,8 +2036,11 @@
       <c r="J24" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="K24" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>141</v>
       </c>
@@ -1984,8 +2071,11 @@
       <c r="J25" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="204" x14ac:dyDescent="0.2">
+      <c r="K25" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="204" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>151</v>
       </c>
@@ -2016,8 +2106,11 @@
       <c r="J26" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="153" x14ac:dyDescent="0.2">
+      <c r="K26" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="153" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>152</v>
       </c>
@@ -2045,8 +2138,11 @@
       <c r="J27" s="2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="119" x14ac:dyDescent="0.2">
+      <c r="K27" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>157</v>
       </c>
@@ -2077,8 +2173,11 @@
       <c r="J28" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="204" x14ac:dyDescent="0.2">
+      <c r="K28" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="204" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>162</v>
       </c>
@@ -2106,8 +2205,11 @@
       <c r="J29" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="187" x14ac:dyDescent="0.2">
+      <c r="K29" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="187" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>166</v>
       </c>
@@ -2138,8 +2240,11 @@
       <c r="J30" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="255" x14ac:dyDescent="0.2">
+      <c r="K30" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>172</v>
       </c>
@@ -2167,8 +2272,11 @@
       <c r="J31" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+      <c r="K31" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>177</v>
       </c>
@@ -2199,8 +2307,11 @@
       <c r="J32" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="289" x14ac:dyDescent="0.2">
+      <c r="K32" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="289" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>184</v>
       </c>
@@ -2228,8 +2339,11 @@
       <c r="J33" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" ht="187" x14ac:dyDescent="0.2">
+      <c r="K33" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="187" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>188</v>
       </c>
@@ -2257,8 +2371,11 @@
       <c r="J34" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+      <c r="K34" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>191</v>
       </c>
@@ -2289,8 +2406,11 @@
       <c r="J35" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="255" x14ac:dyDescent="0.2">
+      <c r="K35" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>196</v>
       </c>
@@ -2318,8 +2438,11 @@
       <c r="J36" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="221" x14ac:dyDescent="0.2">
+      <c r="K36" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="221" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>201</v>
       </c>
@@ -2350,8 +2473,11 @@
       <c r="J37" s="2" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+      <c r="K37" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>207</v>
       </c>
@@ -2379,8 +2505,11 @@
       <c r="J38" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" ht="238" x14ac:dyDescent="0.2">
+      <c r="K38" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>212</v>
       </c>
@@ -2411,8 +2540,11 @@
       <c r="J39" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" ht="187" x14ac:dyDescent="0.2">
+      <c r="K39" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="187" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>218</v>
       </c>
@@ -2443,8 +2575,11 @@
       <c r="J40" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="238" x14ac:dyDescent="0.2">
+      <c r="K40" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="238" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>223</v>
       </c>
@@ -2475,8 +2610,11 @@
       <c r="J41" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" ht="153" x14ac:dyDescent="0.2">
+      <c r="K41" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="153" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>228</v>
       </c>
@@ -2504,8 +2642,11 @@
       <c r="J42" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+      <c r="K42" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>233</v>
       </c>
@@ -2533,8 +2674,11 @@
       <c r="J43" s="2" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="K43" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>238</v>
       </c>
@@ -2565,8 +2709,11 @@
       <c r="J44" s="2" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="255" x14ac:dyDescent="0.2">
+      <c r="K44" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="255" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>244</v>
       </c>
@@ -2594,8 +2741,11 @@
       <c r="J45" s="2" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="204" x14ac:dyDescent="0.2">
+      <c r="K45" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="204" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>249</v>
       </c>
@@ -2623,8 +2773,11 @@
       <c r="J46" s="2" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" ht="272" x14ac:dyDescent="0.2">
+      <c r="K46" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>254</v>
       </c>
@@ -2651,6 +2804,9 @@
       </c>
       <c r="J47" s="2" t="s">
         <v>256</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>